<commit_message>
Update score lab 2 OOP
</commit_message>
<xml_diff>
--- a/IT002-OOP/it002m22/it002m221.xlsx
+++ b/IT002-OOP/it002m22/it002m221.xlsx
@@ -487,7 +487,9 @@
       <c r="C3" t="n">
         <v>800</v>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>600</v>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -504,7 +506,9 @@
       <c r="C4" t="n">
         <v>800</v>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>800</v>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -566,7 +570,9 @@
       <c r="C8" t="n">
         <v>800</v>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>785.71</v>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -598,7 +604,9 @@
       <c r="C10" t="n">
         <v>800</v>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>800</v>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
@@ -615,7 +623,9 @@
       <c r="C11" t="n">
         <v>800</v>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>800</v>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -632,7 +642,9 @@
       <c r="C12" t="n">
         <v>800</v>
       </c>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>800</v>
+      </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -649,7 +661,9 @@
       <c r="C13" t="n">
         <v>800</v>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>800</v>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
@@ -666,7 +680,9 @@
       <c r="C14" t="n">
         <v>800</v>
       </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>800</v>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
@@ -681,7 +697,9 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>300</v>
+      </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
@@ -713,7 +731,9 @@
       <c r="C17" t="n">
         <v>800</v>
       </c>
-      <c r="D17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>600</v>
+      </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
@@ -730,7 +750,9 @@
       <c r="C18" t="n">
         <v>800</v>
       </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>800</v>
+      </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -747,7 +769,9 @@
       <c r="C19" t="n">
         <v>775</v>
       </c>
-      <c r="D19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>800</v>
+      </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -764,7 +788,9 @@
       <c r="C20" t="n">
         <v>800</v>
       </c>
-      <c r="D20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>600</v>
+      </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
@@ -779,7 +805,9 @@
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>400</v>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
@@ -796,7 +824,9 @@
       <c r="C22" t="n">
         <v>700</v>
       </c>
-      <c r="D22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>500</v>
+      </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
@@ -813,7 +843,9 @@
       <c r="C23" t="n">
         <v>800</v>
       </c>
-      <c r="D23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>800</v>
+      </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -845,7 +877,9 @@
       <c r="C25" t="n">
         <v>750</v>
       </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>600</v>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -862,7 +896,9 @@
       <c r="C26" t="n">
         <v>800</v>
       </c>
-      <c r="D26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>800</v>
+      </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
@@ -909,7 +945,9 @@
       <c r="C29" t="n">
         <v>800</v>
       </c>
-      <c r="D29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>800</v>
+      </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
@@ -926,7 +964,9 @@
       <c r="C30" t="n">
         <v>800</v>
       </c>
-      <c r="D30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>800</v>
+      </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -943,7 +983,9 @@
       <c r="C31" t="n">
         <v>800</v>
       </c>
-      <c r="D31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>800</v>
+      </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -960,7 +1002,9 @@
       <c r="C32" t="n">
         <v>800</v>
       </c>
-      <c r="D32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>800</v>
+      </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -992,7 +1036,9 @@
       <c r="C34" t="n">
         <v>800</v>
       </c>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>800</v>
+      </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
@@ -1009,7 +1055,9 @@
       <c r="C35" t="n">
         <v>775</v>
       </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>614.29</v>
+      </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -1041,7 +1089,9 @@
       <c r="C37" t="n">
         <v>800</v>
       </c>
-      <c r="D37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>800</v>
+      </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
@@ -1058,7 +1108,9 @@
       <c r="C38" t="n">
         <v>725</v>
       </c>
-      <c r="D38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>800</v>
+      </c>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -1075,7 +1127,9 @@
       <c r="C39" t="n">
         <v>780</v>
       </c>
-      <c r="D39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>800</v>
+      </c>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -1092,7 +1146,9 @@
       <c r="C40" t="n">
         <v>800</v>
       </c>
-      <c r="D40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>771.4299999999999</v>
+      </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
@@ -1109,7 +1165,9 @@
       <c r="C41" t="n">
         <v>800</v>
       </c>
-      <c r="D41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>800</v>
+      </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
@@ -1143,7 +1201,9 @@
       <c r="C43" t="n">
         <v>775</v>
       </c>
-      <c r="D43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>800</v>
+      </c>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
@@ -1160,7 +1220,9 @@
       <c r="C44" t="n">
         <v>800</v>
       </c>
-      <c r="D44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>771.4299999999999</v>
+      </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -1177,7 +1239,9 @@
       <c r="C45" t="n">
         <v>800</v>
       </c>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>800</v>
+      </c>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
@@ -1194,7 +1258,9 @@
       <c r="C46" t="n">
         <v>800</v>
       </c>
-      <c r="D46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>800</v>
+      </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
@@ -1226,7 +1292,9 @@
       <c r="C48" t="n">
         <v>800</v>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>700</v>
+      </c>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>

</xml_diff>